<commit_message>
sunday data rain is falling
</commit_message>
<xml_diff>
--- a/Assets/Studies/CHI26_Study1_Funneling/data_processing/analysis/p5/p5_analysis.xlsx
+++ b/Assets/Studies/CHI26_Study1_Funneling/data_processing/analysis/p5/p5_analysis.xlsx
@@ -5740,7 +5740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5766,7 +5766,12 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>FeltLocation</t>
+          <t>FeltLocation_mean</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>FeltLocation_sem</t>
         </is>
       </c>
     </row>
@@ -5783,6 +5788,9 @@
       <c r="D2" t="n">
         <v>0.126326685</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.110171315</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -5797,6 +5805,9 @@
       <c r="D3" t="n">
         <v>0.06619815</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.03908652154687299</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -5810,6 +5821,9 @@
       </c>
       <c r="D4" t="n">
         <v>0.146398175</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.08103833338678147</v>
       </c>
     </row>
     <row r="5">
@@ -5825,6 +5839,9 @@
       <c r="D5" t="n">
         <v>0.4235934825</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.2157364296148972</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -5839,6 +5856,9 @@
       <c r="D6" t="n">
         <v>0.108026825</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.06591565264255492</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -5853,6 +5873,9 @@
       <c r="D7" t="n">
         <v>0.09218947499999999</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.05294134990086616</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -5867,6 +5890,9 @@
       <c r="D8" t="n">
         <v>0.7022332999999999</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.1951076997441413</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -5881,6 +5907,9 @@
       <c r="D9" t="n">
         <v>0.625568025</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.1358648912345851</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -5895,6 +5924,9 @@
       <c r="D10" t="n">
         <v>0.731700225</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.103304458405211</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -5909,6 +5941,9 @@
       <c r="D11" t="n">
         <v>0.8362771333333333</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.08770418712734175</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -5923,6 +5958,9 @@
       <c r="D12" t="n">
         <v>0.8924137</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.03491347755397142</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -5937,6 +5975,9 @@
       <c r="D13" t="n">
         <v>0.93172565</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.04029213953425036</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -5951,6 +5992,9 @@
       <c r="D14" t="n">
         <v>0.9883876333333333</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.004543166666666654</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -5965,6 +6009,9 @@
       <c r="D15" t="n">
         <v>0.875</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -5978,6 +6025,9 @@
       </c>
       <c r="D16" t="n">
         <v>0.995961075</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.004038924999999998</v>
       </c>
     </row>
   </sheetData>
@@ -5986,6 +6036,608 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Temperature</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>FeltLocation_mean</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>FeltLocation_sem</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1547213133333334</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.07350219628285615</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.12084311</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0253547637660217</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.162103905</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.04399245149670595</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.262052925</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.08140434709843383</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2495594925</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0938993718398614</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1114978475</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0613428999862325</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8590354</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1206212465522831</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5494067</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1615808256107296</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.734539725</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1305259416407927</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.9049073750000001</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.02919907643785944</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9646635</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.02204273727897695</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.95841665</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.02526908665852078</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.969206525</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.02376171338888728</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9238431</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.03774461303435674</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9367730249999999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.02728231192520089</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Temperature</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>FeltLocation_mean</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>FeltLocation_sem</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.08259891750000001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.01725933582406557</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.086510475</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.02915320620593256</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.07200430025</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.04017178979663463</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.171758025</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.06011087313284629</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1229193225</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.02451828750385665</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.3472368175</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0966035480163029</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.79820725</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1057900180329608</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.52839465</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.07145830211582019</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.790761125</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1432080587623498</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.92888615</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.06511646377055884</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.812340925</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.05550644451455427</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.7188976</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.1736949542517715</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9539371249999999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.046062875</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.91462515</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.03463314494889013</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.98176385</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.01823615000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6012,12 +6664,12 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Duration</t>
+          <t>FeltLocation_mean</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>FeltLocation</t>
+          <t>FeltLocation_sem</t>
         </is>
       </c>
     </row>
@@ -6029,10 +6681,10 @@
         <v>-15</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.1163569977777778</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1547213133333334</v>
+        <v>0.03105509752217602</v>
       </c>
     </row>
     <row r="3">
@@ -6043,10 +6695,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.09118391166666667</v>
       </c>
       <c r="D3" t="n">
-        <v>0.12084311</v>
+        <v>0.01791172485067583</v>
       </c>
     </row>
     <row r="4">
@@ -6057,10 +6709,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.1268354600833333</v>
       </c>
       <c r="D4" t="n">
-        <v>0.162103905</v>
+        <v>0.0325585621551735</v>
       </c>
     </row>
     <row r="5">
@@ -6071,10 +6723,10 @@
         <v>-15</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.2858014775</v>
       </c>
       <c r="D5" t="n">
-        <v>0.262052925</v>
+        <v>0.07841287676813033</v>
       </c>
     </row>
     <row r="6">
@@ -6085,10 +6737,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.1601685466666667</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2495594925</v>
+        <v>0.04022148535914662</v>
       </c>
     </row>
     <row r="7">
@@ -6099,10 +6751,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.18364138</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1114978475</v>
+        <v>0.05164727619696929</v>
       </c>
     </row>
     <row r="8">
@@ -6113,10 +6765,10 @@
         <v>-15</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.7864919833333333</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8590354</v>
+        <v>0.07860977714961188</v>
       </c>
     </row>
     <row r="9">
@@ -6127,10 +6779,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.5677897916666667</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5494067</v>
+        <v>0.06836843191938237</v>
       </c>
     </row>
     <row r="10">
@@ -6141,10 +6793,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0.7523336916666666</v>
       </c>
       <c r="D10" t="n">
-        <v>0.734539725</v>
+        <v>0.06671312960031939</v>
       </c>
     </row>
     <row r="11">
@@ -6155,10 +6807,10 @@
         <v>-15</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0.8949095909090908</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9049073750000001</v>
+        <v>0.03338423279515879</v>
       </c>
     </row>
     <row r="12">
@@ -6169,10 +6821,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0.8898060416666667</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9646635</v>
+        <v>0.02805226666324806</v>
       </c>
     </row>
     <row r="13">
@@ -6183,10 +6835,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0.8696799666666667</v>
       </c>
       <c r="D13" t="n">
-        <v>0.95841665</v>
+        <v>0.06318681993151082</v>
       </c>
     </row>
     <row r="14">
@@ -6197,10 +6849,10 @@
         <v>-15</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0.9688852272727272</v>
       </c>
       <c r="D14" t="n">
-        <v>0.969206525</v>
+        <v>0.01768305799321687</v>
       </c>
     </row>
     <row r="15">
@@ -6211,10 +6863,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0.9044894166666667</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9238431</v>
+        <v>0.04122894521269786</v>
       </c>
     </row>
     <row r="16">
@@ -6225,462 +6877,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0.9714993166666667</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9367730249999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Temperature</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Duration</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>FeltLocation</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.08259891750000001</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.086510475</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>9</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.07200430025</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.171758025</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1229193225</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.3472368175</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B8" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.79820725</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.52839465</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.790761125</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B11" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.92888615</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.812340925</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B13" t="n">
-        <v>9</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.7188976</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.9539371249999999</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.91462515</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" t="n">
-        <v>9</v>
-      </c>
-      <c r="C16" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.98176385</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Temperature</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>FeltLocation</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1163569977777778</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.09118391166666667</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>9</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.1268354600833333</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.2858014775</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1601685466666667</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.18364138</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B8" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.7864919833333333</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.5677897916666667</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.7523336916666666</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B11" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.8949095909090908</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.8898060416666667</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B13" t="n">
-        <v>9</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.8696799666666667</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" t="n">
-        <v>-15</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.9688852272727272</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.9044894166666667</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" t="n">
-        <v>9</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.9714993166666667</v>
+        <v>0.01253992107185321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>